<commit_message>
bug fix (column location)
</commit_message>
<xml_diff>
--- a/playground_data/result/fmt_seg_B_CDC記者會textdate.xlsx
+++ b/playground_data/result/fmt_seg_B_CDC記者會textdate.xlsx
@@ -441,27 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>seg_B</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>report</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>備註</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>seg_B</t>
         </is>
       </c>
     </row>
@@ -471,15 +471,16 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
         <v>12</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>2021-01-06</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">我們各位好朋友們大家午安
 謝謝大家今天來參加我們指揮中心的記者會
@@ -1012,12 +1013,7 @@
 </t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1025,21 +1021,17 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
         <v>34</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2021-01-07</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1047,21 +1039,17 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
         <v>56</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>2021-01-08</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1069,21 +1057,17 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
         <v>78</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>2021-01-09</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1091,21 +1075,17 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
         <v>90</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>2021-01-10</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1113,21 +1093,17 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
         <v>23</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>2021-01-11</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1135,15 +1111,16 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
         <v>45</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>2021-01-12</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>我們各位好朋友們 大家午安 謝謝大家
 來參加今天的記者會  也等了一下子 那
@@ -1351,12 +1328,7 @@
 今天就先跟大家報告到這裡</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>